<commit_message>
26 Aug 2025 Dorm
</commit_message>
<xml_diff>
--- a/KiCads/kicad_upwork/jonathan/touch_switch/touch_switch.xlsx
+++ b/KiCads/kicad_upwork/jonathan/touch_switch/touch_switch.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haque\Documents\KiCad\7.0\projects\kicad_upwork\jonathan\touch_switch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\kicads\jonathan\touch_switch\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23750" windowHeight="9970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23750" windowHeight="9520"/>
   </bookViews>
   <sheets>
     <sheet name="touch_switch" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
   <si>
     <t>Item</t>
   </si>
@@ -39,21 +39,6 @@
     <t>Footprint</t>
   </si>
   <si>
-    <t>Datasheet</t>
-  </si>
-  <si>
-    <t>DNP</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>LIB</t>
-  </si>
-  <si>
-    <t>MF</t>
-  </si>
-  <si>
     <t>MP</t>
   </si>
   <si>
@@ -78,9 +63,6 @@
     <t>Capacitor_SMD:C_0805_2012Metric</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
     <t>C2</t>
   </si>
   <si>
@@ -126,9 +108,6 @@
     <t>Connector_USB:USB_B_Lumberg_2411_02_Horizontal</t>
   </si>
   <si>
-    <t xml:space="preserve"> ~</t>
-  </si>
-  <si>
     <t>5405-241106-ND</t>
   </si>
   <si>
@@ -165,7 +144,10 @@
     <t>R2</t>
   </si>
   <si>
-    <t>Device:R</t>
+    <t>Device:R_Small</t>
+  </si>
+  <si>
+    <t>CR0805-JW-331ELFTR-ND</t>
   </si>
   <si>
     <t>U1</t>
@@ -180,12 +162,6 @@
     <t>TTP223-BA6:SOT23-6</t>
   </si>
   <si>
-    <t>CID</t>
-  </si>
-  <si>
-    <t>tontek</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -193,6 +169,21 @@
   </si>
   <si>
     <t>C42422127</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>H11F1S</t>
+  </si>
+  <si>
+    <t>touch_switch:H11F1S</t>
+  </si>
+  <si>
+    <t>H11F1SM:OPTOCOUPLER_H11F3SR2M</t>
+  </si>
+  <si>
+    <t>H11F1SM-ND</t>
   </si>
 </sst>
 </file>
@@ -999,18 +990,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="16.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" customWidth="1"/>
+    <col min="5" max="5" width="29.54296875" customWidth="1"/>
+    <col min="6" max="6" width="47.453125" customWidth="1"/>
+    <col min="7" max="7" width="16.90625" customWidth="1"/>
+    <col min="8" max="8" width="15.90625" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" customWidth="1"/>
+    <col min="10" max="10" width="26.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1041,23 +1038,8 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1065,22 +1047,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1088,28 +1067,25 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
         <v>19</v>
       </c>
-      <c r="N3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1117,28 +1093,25 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
         <v>24</v>
       </c>
-      <c r="O4" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1146,28 +1119,25 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" t="s">
-        <v>24</v>
-      </c>
-      <c r="O5" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1175,28 +1145,25 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" t="s">
-        <v>24</v>
-      </c>
-      <c r="O6" t="s">
-        <v>41</v>
+        <v>33</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1204,28 +1171,25 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O7" t="s">
-        <v>46</v>
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1233,28 +1197,22 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="D8">
+        <v>330</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" t="s">
-        <v>19</v>
-      </c>
-      <c r="N8" t="s">
-        <v>24</v>
-      </c>
-      <c r="O8" t="s">
-        <v>46</v>
+        <v>38</v>
+      </c>
+      <c r="J8" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1262,34 +1220,51 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" t="s">
         <v>49</v>
       </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
         <v>50</v>
       </c>
-      <c r="E9" t="s">
+      <c r="D10" t="s">
         <v>51</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E10" t="s">
         <v>52</v>
       </c>
-      <c r="J9" t="s">
+      <c r="F10" t="s">
         <v>53</v>
       </c>
-      <c r="K9" t="s">
+      <c r="J10" t="s">
         <v>54</v>
-      </c>
-      <c r="L9" t="s">
-        <v>50</v>
-      </c>
-      <c r="M9" t="s">
-        <v>55</v>
-      </c>
-      <c r="N9" t="s">
-        <v>56</v>
-      </c>
-      <c r="O9" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>